<commit_message>
Get only unique countries.
</commit_message>
<xml_diff>
--- a/data/whitelists/extraction/country_groups.xlsx
+++ b/data/whitelists/extraction/country_groups.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Australia, New Zealand</t>
+          <t>New Zealand, Australia</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Australia, New Zealand</t>
+          <t>New Zealand, Australia</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -630,7 +630,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Hong Kong, Singapore, South Korea, Taiwan, Hong Kong</t>
+          <t>Hong Kong, South Korea, Taiwan, Singapore</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -647,7 +647,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>North Africa, Arabia, Algeria, Bahrain, Comoros, Djibouti, Egypt, Iraq, Jordan, Kuwait, Lebanon, Libya, Mauritania, Morocco, Oman, Palestine, Qatar, Saudi Arabia, Somalia, Sudan, Syria, Tunisia, United Arab Emirates, Yemen</t>
+          <t>Palestine, North Africa, Algeria, Bahrain, Libya, Morocco, Arabia, Qatar, Somalia, Djibouti, Mauritania, United Arab Emirates, Sudan, Lebanon, Iraq, Comoros, Oman, Tunisia, Syria, Kuwait, Saudi Arabia, Jordan, Yemen, Egypt</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Japan, India, China, Australia, South Korea, New Zealand</t>
+          <t>South Korea, Japan, New Zealand, India, China, Australia</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Estonia, Latvia, Lithuania</t>
+          <t>Lithuania, Latvia, Estonia</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Brazil, South Africa, India, China</t>
+          <t>Brazil, India, South Africa, China</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Belgium, Luxembourg</t>
+          <t>Luxembourg, Belgium</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -788,7 +788,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>France, Germany, Italy, Spain</t>
+          <t>Italy, Germany, France, Spain</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -805,7 +805,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Bangladesh, Bhutan, India, Myanmar, Nepal, Sri Lanka, Thailand</t>
+          <t>India, Myanmar, Sri Lanka, Bhutan, Thailand, Nepal, Bangladesh</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -822,7 +822,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Brazil, Russia, India, China</t>
+          <t>Brazil, India, Russia, China</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Brazil, Russia, India, China, South Africa</t>
+          <t>India, China, Brazil, Russia, South Africa</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -895,7 +895,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Canada, Australia, New Zealand</t>
+          <t>New Zealand, Canada, Australia</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Montenegro, Serbia, Albania, Bosnia-Herzegovina, Moldova, North Macedonia, Kosovo</t>
+          <t>Serbia, Montenegro, Kosovo, Bosnia-Herzegovina, North Macedonia, Albania, Moldova</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -955,7 +955,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Colombia, Indonesia, Vietnam, Egypt, Turkey, South Africa</t>
+          <t>Colombia, Vietnam, Indonesia, Egypt, Turkey, South Africa</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -972,7 +972,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Cambodia, Laos, Myanmar, Vietnam</t>
+          <t>Vietnam, Myanmar, Cambodia, Laos</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -989,7 +989,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Bulgaria, Cuba, Czechoslovakia, East Germany, Hungary, Mongolia, Poland, Romania, Vietnam</t>
+          <t>Hungary, Vietnam, Czechoslovakia, Cuba, Romania, Bulgaria, East Germany, Poland, Mongolia</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Republics, Russia, Armenia, Azerbaijan, Belarus, Moldova, Kazakhstan, Kyrgyzstan, Tajikistan, Turkmenistan, Uzbekistan</t>
+          <t>Kyrgyzstan, Kazakhstan, Uzbekistan, Republics, Armenia, Azerbaijan, Belarus, Tajikistan, Russia, Turkmenistan, Moldova</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Russia, Armenia, Belarus, Kazakhstan, Kyrgyzstan, Tajikistan, Serbia, Afghanistan</t>
+          <t>Kyrgyzstan, Serbia, Kazakhstan, Armenia, Belarus, Tajikistan, Russia, Afghanistan</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1126,7 +1126,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Australia, Iceland, New Zealand, South Korea, Austria, Finland, Ireland, Norway, Spain, Belgium, France, Italy, Poland, Sweden, Canada, Germany, Japan, Portugal, Switzerland, Czech Republic, Greece, Luxembourg, Slovakia, United Kingdom, Denmark, Hungary, Netherlands, Slovenia, United States</t>
+          <t>New Zealand, Slovakia, Denmark, Finland, Ireland, Portugal, Luxembourg, Japan, Belgium, Czech Republic, Slovenia, Poland, Italy, Canada, Sweden, Switzerland, Hungary, Netherlands, Austria, Iceland, Australia, United States, South Korea, France, Norway, Spain, Greece, United Kingdom, Germany</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Germany, Austria, Switzerland, Germany, Austria, Austria, Switzerland</t>
+          <t>Austria, Germany, Switzerland</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Germany, Austria, Switzerland</t>
+          <t>Austria, Germany, Switzerland</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Burundi, Kenya, Rwanda, South Sudan, Tanzania, Uganda</t>
+          <t>South Sudan, Tanzania, Burundi, Uganda, Kenya, Rwanda</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Armenia, Azerbaijan, Belarus, Georgia, Moldova, Ukraine</t>
+          <t>Ukraine, Armenia, Azerbaijan, Belarus, Moldova, Georgia</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Afghanistan, Azerbaijan, Iran, Kazakhstan, Kyrgyzstan, Pakistan, Tajikistan, Turkey, Turkmenistan, Uzbekistan</t>
+          <t>Kyrgyzstan, Turkmenistan, Kazakhstan, Uzbekistan, Iran, Azerbaijan, Turkey, Tajikistan, Afghanistan, Pakistan</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Belarus, Kazakhstan, Russia, Armenia, Kyrgyzstan, Moldova, Uzbekistan, Cuba</t>
+          <t>Kyrgyzstan, Cuba, Kazakhstan, Uzbekistan, Armenia, Belarus, Russia, Moldova</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Australia, Canada, New Zealand</t>
+          <t>New Zealand, Canada, Australia</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1387,7 +1387,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Hong Kong, Singapore, South Korea, Taiwan</t>
+          <t>Hong Kong, South Korea, Taiwan, Singapore</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>France, Italy</t>
+          <t>Italy, France</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>France, Italy, Spain</t>
+          <t>Italy, France, Spain</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Brazil, Germany, India, Japan</t>
+          <t>Brazil, India, Germany, Japan</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Germany, Italy, Poland, Spain</t>
+          <t>Poland, Italy, Germany, Spain</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Canada, France, Germany, Italy, Japan</t>
+          <t>France, Japan, Italy, Germany, Canada</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1562,7 +1562,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Brazil, China, India, Mexico, South Africa</t>
+          <t>India, China, Brazil, Mexico, South Africa</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Argentina, Australia, Brazil, Canada, China, France, Germany, India, Indonesia, Italy, Japan, South Korea, Mexico, Russia, Saudi Arabia, South Africa, Turkey, United Kingdom, United States</t>
+          <t>India, Argentina, Japan, Indonesia, Turkey, Mexico, Italy, Canada, Australia, Brazil, United States, Russia, South Korea, Saudi Arabia, France, United Kingdom, China, South Africa, Germany</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Georgia, Ukraine, Azerbaijan, Moldova</t>
+          <t>Moldova, Ukraine, Azerbaijan, Georgia</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Bahrain, Kuwait, Oman, Qatar, Saudi Arabia, UAE, Iraq</t>
+          <t>Kuwait, Iraq, Saudi Arabia, Bahrain, Oman, Qatar, UAE</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>China, China, Hong Kong, Macau, Taiwan</t>
+          <t>Hong Kong, China, Taiwan, Macau</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Germany, Austria, Switzerland</t>
+          <t>Austria, Germany, Switzerland</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>India, Brazil, South Africa</t>
+          <t>Brazil, India, South Africa</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Israel, Jordan, Lebanon, Palestine, Syria</t>
+          <t>Palestine, Israel, Jordan, Lebanon, Syria</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Argentina, Brazil, Paraguay, Uruguay</t>
+          <t>Brazil, Argentina, Uruguay, Paraguay</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Mexico, Indonesia, Republic of Korea, Turkey, Australia</t>
+          <t>Indonesia, Republic of Korea, Turkey, Australia, Mexico</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -1848,7 +1848,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Mexico, Indonesia, Nigeria, Turkey</t>
+          <t>Mexico, Turkey, Nigeria, Indonesia</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Canada, Mexico</t>
+          <t>Mexico, Canada</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2028,7 +2028,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Bangladesh, Egypt, Indonesia, Iran, Mexico, Nigeria, Pakistan, Philippines, Turkey, South Korea, Vietnam</t>
+          <t>South Korea, Vietnam, Indonesia, Nigeria, Egypt, Philippines, Iran, Turkey, Bangladesh, Mexico, Pakistan</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Canada, United States, Mexico</t>
+          <t>Mexico, United States, Canada</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2088,7 +2088,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Denmark, Norway, Sweden, Finland, Iceland</t>
+          <t>Sweden, Norway, Denmark, Finland, Iceland</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2196,7 +2196,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>China, France, Russia</t>
+          <t>Russia, China, France</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Chile, Colombia, Mexico, Peru</t>
+          <t>Colombia, Mexico, Chile, Peru</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Chile, Colombia, Mexico, Peru</t>
+          <t>Colombia, Mexico, Chile, Peru</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2264,7 +2264,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Portugal, Greece, Spain, Italy, Ireland</t>
+          <t>Ireland, Portugal, Spain, Greece, Italy</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -2337,7 +2337,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Denmark, Norway, Sweden, Finland, Sweden</t>
+          <t>Norway, Sweden, Denmark, Finland</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -2354,7 +2354,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>China, Kazakhstan, Kyrgyzstan, Russia, Tajikistan, Uzbekistan, India, Pakistan</t>
+          <t>Kyrgyzstan, India, Kazakhstan, Uzbekistan, China, Tajikistan, Russia, Pakistan</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -2371,7 +2371,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Saarland, Lorraine, Luxembourg</t>
+          <t>Luxembourg, Lorraine, Saarland</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Argentina, Chile, Paraguay, Uruguay</t>
+          <t>Argentina, Uruguay, Chile, Paraguay</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2418,7 +2418,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Afghanistan, Bangladesh, Bhutan, Maldives, Nepal, India, Pakistan, Sri Lanka</t>
+          <t>India, Sri Lanka, Bhutan, Maldives, Nepal, Bangladesh, Afghanistan, Pakistan</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Indonesia, Malaysia, Philippines, Thailand, Vietnam</t>
+          <t>Vietnam, Indonesia, Philippines, Thailand, Malaysia</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Turkey, Azerbaijan, Kazakhstan, Uzbekistan, Kyrgyzstan, Hungary</t>
+          <t>Kyrgyzstan, Hungary, Kazakhstan, Uzbekistan, Azerbaijan, Turkey</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -2469,7 +2469,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>United Kingdom, UK, England, Scotland, Wales, Northern Ireland</t>
+          <t>Wales, UK, Northern Ireland, United Kingdom, Scotland, England</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -2516,7 +2516,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Hungary, Poland, Slovakia</t>
+          <t>Poland, Slovakia, Hungary</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Vietnam, Indonesia, South Africa, Turkey, Argentina</t>
+          <t>Vietnam, Indonesia, Argentina, Turkey, South Africa</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">

</xml_diff>